<commit_message>
Clean up input file
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anarion\Documents\repos\sankey-finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818F9C16-07C1-4BA0-B3F8-CBD72D49DEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5747F2-4E94-42BD-A33A-3941B5E2F93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34410" yWindow="345" windowWidth="17190" windowHeight="10500" xr2:uid="{57BD4CDB-73B4-4590-968C-CCB92BA6CDD1}"/>
+    <workbookView xWindow="34410" yWindow="345" windowWidth="17190" windowHeight="10500" activeTab="2" xr2:uid="{57BD4CDB-73B4-4590-968C-CCB92BA6CDD1}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
     <sheet name="links" sheetId="2" r:id="rId2"/>
-    <sheet name="metadata" sheetId="3" r:id="rId3"/>
-    <sheet name="currency" sheetId="4" r:id="rId4"/>
-    <sheet name="abbreviation" sheetId="5" r:id="rId5"/>
+    <sheet name="metadata" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="color">nodes!$C:$C</definedName>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
   <si>
     <t>source</t>
   </si>
@@ -135,9 +133,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>Nokia FY2022 Results</t>
-  </si>
-  <si>
     <t>€</t>
   </si>
   <si>
@@ -151,6 +146,9 @@
   </si>
   <si>
     <t>abbreviation</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -512,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE9EA5F-136E-48E9-AE0C-0FC26DDD0F0A}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="A2:D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +740,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,82 +1008,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CC5BEF-D334-4881-9F98-9D32EE35A52D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96658AF9-DEF6-4DAC-942E-EC6E2364C8B8}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCC0A24-CBF8-485E-BE95-0CDD82205A1B}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4497924A-B605-4972-89B8-5C19855040BA}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>